<commit_message>
Add seed data and update readme for foundry docker compose instructions
</commit_message>
<xml_diff>
--- a/test-data/test-data.xlsx
+++ b/test-data/test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmhaske/Repositories/hl7-davinci-pr/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ADA283-4A4B-704B-A5C6-E66001E39B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40244C2-32D9-DA4E-968D-F767CF5B79B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="39000" windowHeight="23900" xr2:uid="{2778282F-DD2E-9745-BDC4-0769A09CC95F}"/>
+    <workbookView xWindow="42640" yWindow="4840" windowWidth="48420" windowHeight="23900" xr2:uid="{2778282F-DD2E-9745-BDC4-0769A09CC95F}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="79">
   <si>
     <t>provider</t>
   </si>
@@ -339,9 +339,30 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="58">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -368,6 +389,21 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -401,6 +437,27 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -425,12 +482,6 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
@@ -458,33 +509,6 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
@@ -512,6 +536,9 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -524,25 +551,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -582,13 +591,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="50" xr:uid="{71CA5CC3-CE18-7949-9C77-6226D6B03EA6}" name="Table151" displayName="Table151" ref="B8:E9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="50" xr:uid="{71CA5CC3-CE18-7949-9C77-6226D6B03EA6}" name="Table151" displayName="Table151" ref="B8:E9" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <autoFilter ref="B8:E9" xr:uid="{71CA5CC3-CE18-7949-9C77-6226D6B03EA6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2CA2ED96-F1F1-2846-97AD-98C2A9BB0D74}" name="id" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{4A18D903-7258-DA4A-A3D6-B6A4F3738587}" name="provider_npi" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{B244A140-FAC1-014C-942E-D156B9028CAD}" name="tin" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{781C4DED-AFA8-DA43-9A0C-BA3D3082B536}" name="Query" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{2CA2ED96-F1F1-2846-97AD-98C2A9BB0D74}" name="id" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{4A18D903-7258-DA4A-A3D6-B6A4F3738587}" name="provider_npi" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{B244A140-FAC1-014C-942E-D156B9028CAD}" name="tin" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{781C4DED-AFA8-DA43-9A0C-BA3D3082B536}" name="Query" dataDxfId="52">
       <calculatedColumnFormula>_xlfn.CONCAT( "INSERT INTO provider (id, provider_npi, tin) VALUES (", B9,", '", C9,"', '", D9,"');")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -597,14 +606,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="51" xr:uid="{724D2257-0528-6A43-AD71-187D11C1159E}" name="Table252" displayName="Table252" ref="B13:F15" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="51" xr:uid="{724D2257-0528-6A43-AD71-187D11C1159E}" name="Table252" displayName="Table252" ref="B13:F15" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="B13:F15" xr:uid="{724D2257-0528-6A43-AD71-187D11C1159E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{27DBA7CF-AF32-E248-8DC4-994CDC58EE74}" name="id" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{74F7D55D-5941-9B46-9E60-6A5C830109E8}" name="first_name" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{286F2C83-410C-4C43-9BBE-83496279208D}" name="last_name" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{D30C046D-A06F-054D-90E1-EEB5C57596DC}" name="date_of_birth" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{FC0667FC-5ACE-1C4A-802D-BA07C0FAE067}" name="Query" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{27DBA7CF-AF32-E248-8DC4-994CDC58EE74}" name="id" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{74F7D55D-5941-9B46-9E60-6A5C830109E8}" name="first_name" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{286F2C83-410C-4C43-9BBE-83496279208D}" name="last_name" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{D30C046D-A06F-054D-90E1-EEB5C57596DC}" name="date_of_birth" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{FC0667FC-5ACE-1C4A-802D-BA07C0FAE067}" name="Query" dataDxfId="45">
       <calculatedColumnFormula>_xlfn.CONCAT("INSERT INTO patient (id, first_name, last_name, date_of_birth) VALUES (",B14,", '",C14,"', '",D14,"', '",E14,"');")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -613,13 +622,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="52" xr:uid="{5BD26E78-7BC0-354A-AB85-561296C5C055}" name="Table353" displayName="Table353" ref="B19:E21" totalsRowShown="0" headerRowDxfId="6" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="52" xr:uid="{5BD26E78-7BC0-354A-AB85-561296C5C055}" name="Table353" displayName="Table353" ref="B19:E21" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="B19:E21" xr:uid="{5BD26E78-7BC0-354A-AB85-561296C5C055}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E12033D6-6668-2742-8AEC-456C01C8D1FC}" name="id" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{A5C11146-DCD4-EE4D-922F-D94C96DEBDE0}" name="payer_name" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{800DF4E6-3644-6A4D-BCCE-177C23A858AF}" name="payer_identity" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{7EA989B3-F1F9-BA48-8B09-21D863F555BD}" name="Query" dataDxfId="43">
+    <tableColumn id="1" xr3:uid="{E12033D6-6668-2742-8AEC-456C01C8D1FC}" name="id" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{A5C11146-DCD4-EE4D-922F-D94C96DEBDE0}" name="payer_name" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{800DF4E6-3644-6A4D-BCCE-177C23A858AF}" name="payer_identity" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{7EA989B3-F1F9-BA48-8B09-21D863F555BD}" name="Query" dataDxfId="39">
       <calculatedColumnFormula>_xlfn.CONCAT("INSERT INTO payer (id, payer_name, payer_identity) VALUES (",B20,", '",C20,"', '",D20,"');")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -628,14 +637,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="53" xr:uid="{C853C29F-273E-9540-82CF-C4C9F5BED519}" name="Table454" displayName="Table454" ref="B25:E27" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
-  <autoFilter ref="B25:E27" xr:uid="{C853C29F-273E-9540-82CF-C4C9F5BED519}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{04F6DE39-7522-9A4E-925B-0B936CE410F9}" name="patient_id" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{9C2AAC01-ADD7-6141-B787-51DB7A9A989B}" name="payer_id" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{D72859B4-6564-EE49-AC61-D21CD3AB32B7}" name="subscriber_patient_id" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{11B81DA4-A919-9441-9518-EDBA7B3CF2C6}" name="Query" dataDxfId="37">
-      <calculatedColumnFormula>_xlfn.CONCAT("INSERT INTO subscriber_patient (patient_id, payer_id, subscriber_patient_id) VALUES (",B26,", ",C26,", '",D26,"');")</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="53" xr:uid="{C853C29F-273E-9540-82CF-C4C9F5BED519}" name="Table454" displayName="Table454" ref="B25:F27" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+  <autoFilter ref="B25:F27" xr:uid="{C853C29F-273E-9540-82CF-C4C9F5BED519}"/>
+  <tableColumns count="5">
+    <tableColumn id="5" xr3:uid="{C357CC2D-4A2B-2C40-93EA-2DF471F75F48}" name="id" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{04F6DE39-7522-9A4E-925B-0B936CE410F9}" name="patient_id" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{9C2AAC01-ADD7-6141-B787-51DB7A9A989B}" name="payer_id" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{D72859B4-6564-EE49-AC61-D21CD3AB32B7}" name="subscriber_patient_id" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{11B81DA4-A919-9441-9518-EDBA7B3CF2C6}" name="Query" dataDxfId="4">
+      <calculatedColumnFormula>_xlfn.CONCAT("INSERT INTO subscriber_patient (id, patient_id, payer_id, subscriber_patient_id) VALUES (",B26,", ",C26,", ",D26,", '",E26,"');")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -643,22 +653,22 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{9E8B241A-9A09-8148-B336-0201664E5D6F}" name="Table555" displayName="Table555" ref="B31:N34" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{9E8B241A-9A09-8148-B336-0201664E5D6F}" name="Table555" displayName="Table555" ref="B31:N34" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="B31:N34" xr:uid="{9E8B241A-9A09-8148-B336-0201664E5D6F}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{207A742E-61D0-F044-9C85-757C01A68F2F}" name="id" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{E5B0D51E-0587-6041-8B36-1B7C3A655142}" name="received_dt" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{BDCF5823-A80E-4C46-915B-B10CBDCBD8F1}" name="provider_tin" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{CA545A89-E390-CE42-8BDF-A6893CD8BDDA}" name="provider_claimID" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{D3DBA6AD-C660-8843-8841-EFE61F30BB34}" name="provider_npi" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{C2CC1E35-6BA6-CA44-9B70-E75BF5F41F97}" name="payer_claimID" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{284FE521-F75E-A748-8757-3C92C0632225}" name="subscriber_patient_id" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{754B6A09-A2A1-C74A-A3A8-B2AE36E5A428}" name="dos_dt" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{C02B2380-1564-1040-9792-90DD15D0B156}" name="claim_charge_amt" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{645C3A26-AF8C-6140-8ADA-DE862AB9F90F}" name="patient_id" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{15C2BCB3-DEF1-204F-83BA-FC6C9DB446F4}" name="provider_id" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{76E8BCCB-EB38-6640-9F03-EA900165804E}" name="payer_id" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{93424C75-34D7-FE4E-93E9-49AE523CA0BF}" name="Query" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{207A742E-61D0-F044-9C85-757C01A68F2F}" name="id" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{E5B0D51E-0587-6041-8B36-1B7C3A655142}" name="received_dt" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{BDCF5823-A80E-4C46-915B-B10CBDCBD8F1}" name="provider_tin" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{CA545A89-E390-CE42-8BDF-A6893CD8BDDA}" name="provider_claimID" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{D3DBA6AD-C660-8843-8841-EFE61F30BB34}" name="provider_npi" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{C2CC1E35-6BA6-CA44-9B70-E75BF5F41F97}" name="payer_claimID" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{284FE521-F75E-A748-8757-3C92C0632225}" name="subscriber_patient_id" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{754B6A09-A2A1-C74A-A3A8-B2AE36E5A428}" name="dos_dt" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{C02B2380-1564-1040-9792-90DD15D0B156}" name="claim_charge_amt" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{645C3A26-AF8C-6140-8ADA-DE862AB9F90F}" name="patient_id" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{15C2BCB3-DEF1-204F-83BA-FC6C9DB446F4}" name="provider_id" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{76E8BCCB-EB38-6640-9F03-EA900165804E}" name="payer_id" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{93424C75-34D7-FE4E-93E9-49AE523CA0BF}" name="Query" dataDxfId="19">
       <calculatedColumnFormula>_xlfn.CONCAT("INSERT INTO claim_query (id, received_dt, provider_tin, provider_claimID, provider_npi, payer_claimID, subscriber_patient_id, dos_dt, claim_charge_amt, patient_id, provider_id, payer_id) VALUES (",B32,", '",C32,"', '",D32,"', '",E32,"', '",F32,"', '",G32,"', '",H32,"', '",I32,"', ",J32,", ",K32,", ",L32,", ",M32,");")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -667,15 +677,16 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="55" xr:uid="{824A80CA-3FB2-D341-9B3E-B0CF0E4600B1}" name="Table656" displayName="Table656" ref="B38:F41" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="B38:F41" xr:uid="{824A80CA-3FB2-D341-9B3E-B0CF0E4600B1}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3E718CE5-E6FC-234A-9D76-12F3FC6DBF22}" name="claim_id" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{F63E3678-8361-0342-89F1-FB64EAC6137F}" name="payment_number" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{C78A98E2-D7D8-D645-86DF-0ACB95A7C419}" name="amount" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{13B231F6-81DC-F544-868C-4B2EC95208EC}" name="payment_issue_dt" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{AF7B7F29-3FC5-3E42-92B4-BE74B66D479E}" name="Query" dataDxfId="15">
-      <calculatedColumnFormula>_xlfn.CONCAT("INSERT INTO payment (claim_id, payment_number, amount, payment_issue_dt) VALUES (",B39,", '",C39,"', ",D39,", '",E39,"');")</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="55" xr:uid="{824A80CA-3FB2-D341-9B3E-B0CF0E4600B1}" name="Table656" displayName="Table656" ref="B38:G41" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="B38:G41" xr:uid="{824A80CA-3FB2-D341-9B3E-B0CF0E4600B1}"/>
+  <tableColumns count="6">
+    <tableColumn id="6" xr3:uid="{6C0DAC8A-6355-A54C-8EC4-452B540C2F6A}" name="id" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{3E718CE5-E6FC-234A-9D76-12F3FC6DBF22}" name="claim_id" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{F63E3678-8361-0342-89F1-FB64EAC6137F}" name="payment_number" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{C78A98E2-D7D8-D645-86DF-0ACB95A7C419}" name="amount" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{13B231F6-81DC-F544-868C-4B2EC95208EC}" name="payment_issue_dt" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{AF7B7F29-3FC5-3E42-92B4-BE74B66D479E}" name="Query" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT("INSERT INTO payment (id, claim_id, payment_number, amount, payment_issue_dt) VALUES (",B39,", ",C39,", '",D39,"', ",E39,", '",F39,"');")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -683,16 +694,17 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="56" xr:uid="{B65A5118-05A3-CF41-9E4E-CBFB776F3693}" name="Table757" displayName="Table757" ref="B45:G48" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="B45:G48" xr:uid="{B65A5118-05A3-CF41-9E4E-CBFB776F3693}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{97E06704-A08A-484B-9754-13CA51D05754}" name="claim_id" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{E1EE0A25-7EA1-104C-BC87-8F0DF71233D3}" name="remittance_adviceID" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{5F03FB95-3655-9F40-BC88-AFD9C16F909F}" name="remittance_advice_type" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{5878958F-8045-5F41-9D25-B998F07BE04F}" name="remittance_advice_dt" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{12A5BB50-1004-AB44-A80C-7DE899FF5804}" name="remittance_advice_file_size" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{75189044-FA03-B145-AA51-BDEA06B6A1BD}" name="Query" dataDxfId="7">
-      <calculatedColumnFormula>_xlfn.CONCAT("INSERT INTO remittance (claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (",B46,", '",C46,"', '",D46,"', '",E46,"', ",F46,");")</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="56" xr:uid="{B65A5118-05A3-CF41-9E4E-CBFB776F3693}" name="Table757" displayName="Table757" ref="B45:H48" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="B45:H48" xr:uid="{B65A5118-05A3-CF41-9E4E-CBFB776F3693}"/>
+  <tableColumns count="7">
+    <tableColumn id="7" xr3:uid="{751FDD35-153A-AE49-95D4-74CD4783DCA2}" name="id" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{97E06704-A08A-484B-9754-13CA51D05754}" name="claim_id" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{E1EE0A25-7EA1-104C-BC87-8F0DF71233D3}" name="remittance_adviceID" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{5F03FB95-3655-9F40-BC88-AFD9C16F909F}" name="remittance_advice_type" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{5878958F-8045-5F41-9D25-B998F07BE04F}" name="remittance_advice_dt" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{12A5BB50-1004-AB44-A80C-7DE899FF5804}" name="remittance_advice_file_size" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{75189044-FA03-B145-AA51-BDEA06B6A1BD}" name="Query" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("INSERT INTO remittance (id, claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (",B46,", ",C46,", '",D46,"', '",E46,"', '",F46,"', ",G46,");")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1018,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BC94C9-6F11-AB49-BABC-9E1E0F8A0BCB}">
   <dimension ref="A2:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1098,7 +1110,7 @@
       <c r="D9" s="1">
         <v>123456789</v>
       </c>
-      <c r="E9" s="5" t="str">
+      <c r="E9" t="str">
         <f>_xlfn.CONCAT( "INSERT INTO provider (id, provider_npi, tin) VALUES (", B9,", '", C9,"', '", D9,"');")</f>
         <v>INSERT INTO provider (id, provider_npi, tin) VALUES (1, 'PB654', '123456789');</v>
       </c>
@@ -1116,7 +1128,7 @@
       <c r="D10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="5" t="str">
+      <c r="E10" t="str">
         <f>_xlfn.CONCAT( "INSERT INTO provider (id, provider_npi, tin) VALUES (", B10,", '", C10,"', '", D10,"');")</f>
         <v>INSERT INTO provider (id, provider_npi, tin) VALUES (2, 'PB655', '123485858');</v>
       </c>
@@ -1257,15 +1269,18 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1280,11 +1295,14 @@
         <v>56</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO subscriber_patient (patient_id, payer_id, subscriber_patient_id) VALUES (",B26,", ",C26,", '",D26,"');")</f>
-        <v>INSERT INTO subscriber_patient (patient_id, payer_id, subscriber_patient_id) VALUES (1, 1, 'M12345678901');</v>
+      <c r="F26" s="5" t="str">
+        <f t="shared" ref="F26:F27" si="0">_xlfn.CONCAT("INSERT INTO subscriber_patient (id, patient_id, payer_id, subscriber_patient_id) VALUES (",B26,", ",C26,", ",D26,", '",E26,"');")</f>
+        <v>INSERT INTO subscriber_patient (id, patient_id, payer_id, subscriber_patient_id) VALUES (1, 1, 1, 'M12345678901');</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -1298,11 +1316,14 @@
         <v>51</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO subscriber_patient (patient_id, payer_id, subscriber_patient_id) VALUES (",B27,", ",C27,", '",D27,"');")</f>
-        <v>INSERT INTO subscriber_patient (patient_id, payer_id, subscriber_patient_id) VALUES (2, 2, 'M12345513215');</v>
+      <c r="F27" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO subscriber_patient (id, patient_id, payer_id, subscriber_patient_id) VALUES (2, 2, 2, 'M12345513215');</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -1509,18 +1530,21 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1532,17 +1556,20 @@
         <v>56</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F39" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO payment (claim_id, payment_number, amount, payment_issue_dt) VALUES (",B39,", '",C39,"', ",D39,", '",E39,"');")</f>
-        <v>INSERT INTO payment (claim_id, payment_number, amount, payment_issue_dt) VALUES (1, 'A123456', 20.00, '2023-10-02');</v>
+      <c r="G39" s="5" t="str">
+        <f t="shared" ref="G39:G41" si="1">_xlfn.CONCAT("INSERT INTO payment (id, claim_id, payment_number, amount, payment_issue_dt) VALUES (",B39,", ",C39,", '",D39,"', ",E39,", '",F39,"');")</f>
+        <v>INSERT INTO payment (id, claim_id, payment_number, amount, payment_issue_dt) VALUES (1, 1, 'A123456', 20.00, '2023-10-02');</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
@@ -1553,17 +1580,20 @@
         <v>51</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F40" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO payment (claim_id, payment_number, amount, payment_issue_dt) VALUES (",B40,", '",C40,"', ",D40,", '",E40,"');")</f>
-        <v>INSERT INTO payment (claim_id, payment_number, amount, payment_issue_dt) VALUES (2, 'A12385858', 30.00, '2023-11-02');</v>
+      <c r="G40" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO payment (id, claim_id, payment_number, amount, payment_issue_dt) VALUES (2, 2, 'A12385858', 30.00, '2023-11-02');</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -1574,17 +1604,20 @@
         <v>48</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F41" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO payment (claim_id, payment_number, amount, payment_issue_dt) VALUES (",B41,", '",C41,"', ",D41,", '",E41,"');")</f>
-        <v>INSERT INTO payment (claim_id, payment_number, amount, payment_issue_dt) VALUES (3, 'A12385859', 30.00, '2023-11-03');</v>
+      <c r="G41" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO payment (id, claim_id, payment_number, amount, payment_issue_dt) VALUES (3, 3, 'A12385859', 30.00, '2023-11-03');</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
@@ -1599,21 +1632,24 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="G45" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="H45" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1625,20 +1661,23 @@
         <v>56</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="1">
+      <c r="E46" s="1">
         <v>835</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="1">
+      <c r="G46" s="1">
         <v>1024</v>
       </c>
-      <c r="G46" s="1" t="str">
-        <f t="shared" ref="G46" si="0">_xlfn.CONCAT("INSERT INTO remittance (claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (",B46,", '",C46,"', '",D46,"', '",E46,"', ",F46,");")</f>
-        <v>INSERT INTO remittance (claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (1, 'A123456BCD', '835', '2023-10-02', 1024);</v>
+      <c r="H46" s="5" t="str">
+        <f t="shared" ref="H46:H48" si="2">_xlfn.CONCAT("INSERT INTO remittance (id, claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (",B46,", ",C46,", '",D46,"', '",E46,"', '",F46,"', ",G46,");")</f>
+        <v>INSERT INTO remittance (id, claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (1, 1, 'A123456BCD', '835', '2023-10-02', 1024);</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -1649,20 +1688,23 @@
         <v>51</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G47" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO remittance (claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (",B47,", '",C47,"', '",D47,"', '",E47,"', ",F47,");")</f>
-        <v>INSERT INTO remittance (claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (2, 'A123456BCDEF', '835', '2023-11-02', 1536);</v>
+      <c r="H47" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO remittance (id, claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (2, 2, 'A123456BCDEF', '835', '2023-11-02', 1536);</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -1673,20 +1715,23 @@
         <v>48</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D48" s="1">
+      <c r="E48" s="1">
         <v>835</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G48" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO remittance (claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (",B48,", '",C48,"', '",D48,"', '",E48,"', ",F48,");")</f>
-        <v>INSERT INTO remittance (claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (3, 'A123456BCDXY', '835', '2023-11-03', 2048);</v>
+      <c r="H48" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO remittance (id, claim_id, remittance_adviceID, remittance_advice_type, remittance_advice_dt, remittance_advice_file_size) VALUES (3, 3, 'A123456BCDXY', '835', '2023-11-03', 2048);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>